<commit_message>
Update readme & xlsx with products set
</commit_message>
<xml_diff>
--- a/excel/brief_example_with_set.xlsx
+++ b/excel/brief_example_with_set.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZhernokE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB896B7-99E6-4B26-A663-898FEBFB98BD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E562BF7D-E190-4A82-ACDA-788D6F8D30B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="120" windowWidth="20400" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Killing offers " sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Karina Leonova/MSC/RU - Personal View" guid="{EB0EC4D1-8B8D-46FB-BC39-0BA2397624AA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Anna Silnikova/Other/Consultant - Personal View" guid="{89EB5726-03E5-4F2C-A6BE-9D2A424F6109}" mergeInterval="0" personalView="1" xWindow="430" yWindow="70" windowWidth="1329" windowHeight="939" activeSheetId="1"/>
+    <customWorkbookView name="Sofia Sterkhova/MSC/RU - Personal View" guid="{C156F9C8-FAC6-485D-BA71-3158CC8B4510}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="Daria Garshina/MSC/RU - Personal View" guid="{E86FB901-2D43-49F7-AF25-C8E3CE6F969E}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
-    <customWorkbookView name="Sofia Sterkhova/MSC/RU - Personal View" guid="{C156F9C8-FAC6-485D-BA71-3158CC8B4510}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Anna Silnikova/Other/Consultant - Personal View" guid="{89EB5726-03E5-4F2C-A6BE-9D2A424F6109}" mergeInterval="0" personalView="1" xWindow="430" yWindow="70" windowWidth="1329" windowHeight="939" activeSheetId="1"/>
-    <customWorkbookView name="Karina Leonova/MSC/RU - Personal View" guid="{EB0EC4D1-8B8D-46FB-BC39-0BA2397624AA}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -113,12 +113,6 @@
     <t>Универсальный комплексный уход</t>
   </si>
   <si>
-    <t xml:space="preserve">Парфюмироавнный дезодорант-антиперспирант спрей для тела Full Speed Turbo Care (150 мл)
-Гель для бритья  Full Speed Turbo Care (100 мл);Масло для бороды  Full Speed Turbo Care (30 мл);
-Шампунь против перхоти Full Speed Turbo Care (250 мл);Увлажняющий дневной крем для лица SPF 15 для мужчин Full Speed Turbo Care (50 мл);
-</t>
-  </si>
-  <si>
     <t>Парфюмерно-косметический набор Avon Life Colour для него</t>
   </si>
   <si>
@@ -348,6 +342,12 @@
   <si>
     <t>Парфюмерная вода Avon Eve Duet Contrasts Calm;
 Парфюмерная вода Avon Eve Duet Contrasts Daring, 2 x 1,5мл</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Парфюмироавнный дезодорант-антиперспирант спрей для тела Full Speed Turbo Care (150 мл)
+Гель для бритья  Full Speed Turbo Care (100 мл);Масло для бороды  Full Speed Turbo Care (30 мл);
+Шампунь против перхоти Full Speed Turbo Care (250 мл);Увлажняющий дневной крем для лица SPF 15 для мужчин Full Speed Turbo Care (50 мл)
+</t>
   </si>
 </sst>
 </file>
@@ -1084,9 +1084,9 @@
   </sheetPr>
   <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1259,7 @@
         <v>57542</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="27">
         <v>57542</v>
@@ -1308,7 +1308,7 @@
         <v>21</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="H9" s="21"/>
       <c r="I9" s="27">
@@ -1337,14 +1337,14 @@
         <v>1300691</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="21" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21">
@@ -1364,7 +1364,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="16"/>
@@ -1417,7 +1417,7 @@
         <v>1339619</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
@@ -1442,7 +1442,7 @@
         <v>38565</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1479,7 +1479,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -1509,14 +1509,14 @@
         <v>43347</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E19" s="33"/>
       <c r="F19" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="19">
@@ -1529,7 +1529,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -1580,7 +1580,7 @@
         <v>21929</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
@@ -1605,7 +1605,7 @@
         <v>22877</v>
       </c>
       <c r="D23" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E23" s="30"/>
       <c r="F23" s="30"/>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1672,7 +1672,7 @@
         <v>1309663</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
@@ -1697,7 +1697,7 @@
         <v>1309657</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
@@ -1722,7 +1722,7 @@
         <v>1309660</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" s="36"/>
       <c r="F29" s="36"/>
@@ -1747,7 +1747,7 @@
         <v>1309666</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30" s="36"/>
       <c r="F30" s="36"/>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1784,7 +1784,7 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="56"/>
       <c r="C33" s="56"/>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="34" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B34" s="37">
         <v>1198773</v>
@@ -1814,7 +1814,7 @@
         <v>78730</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="35" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="37">
         <v>1189411</v>
@@ -1843,7 +1843,7 @@
         <v>55643</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="36" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36" s="37">
         <v>1198772</v>
@@ -1873,7 +1873,7 @@
         <v>37125</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="37" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="40">
         <v>1200841</v>
@@ -1903,7 +1903,7 @@
         <v>33267</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1945,7 +1945,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="56"/>
       <c r="C40" s="56"/>
@@ -1966,7 +1966,7 @@
     </row>
     <row r="41" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" s="25">
         <v>1175162</v>
@@ -1975,7 +1975,7 @@
         <v>63443</v>
       </c>
       <c r="D41" s="41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E41" s="38"/>
       <c r="F41" s="38"/>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="42" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="25">
         <v>1199750</v>
@@ -2005,7 +2005,7 @@
         <v>52640</v>
       </c>
       <c r="D42" s="41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="38"/>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="43" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" s="25">
         <v>1199766</v>
@@ -2035,7 +2035,7 @@
         <v>62352</v>
       </c>
       <c r="D43" s="41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" s="38"/>
       <c r="F43" s="38"/>
@@ -2056,7 +2056,7 @@
     </row>
     <row r="44" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="25">
         <v>1199789</v>
@@ -2065,7 +2065,7 @@
         <v>71068</v>
       </c>
       <c r="D44" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E44" s="38"/>
       <c r="F44" s="38"/>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="45" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" s="25">
         <v>1200143</v>
@@ -2095,7 +2095,7 @@
         <v>46583</v>
       </c>
       <c r="D45" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E45" s="38"/>
       <c r="F45" s="38"/>
@@ -2116,7 +2116,7 @@
     </row>
     <row r="46" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="25">
         <v>1200145</v>
@@ -2125,7 +2125,7 @@
         <v>47079</v>
       </c>
       <c r="D46" s="41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E46" s="38"/>
       <c r="F46" s="38"/>
@@ -2146,7 +2146,7 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2169,7 +2169,7 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="56"/>
       <c r="C49" s="56"/>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="50" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" s="42">
         <v>1188616</v>
@@ -2201,7 +2201,7 @@
         <v>96008</v>
       </c>
       <c r="D50" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E50" s="38"/>
       <c r="F50" s="38"/>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="51" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B51" s="42">
         <v>1189260</v>
@@ -2231,7 +2231,7 @@
         <v>30940</v>
       </c>
       <c r="D51" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E51" s="38"/>
       <c r="F51" s="38"/>
@@ -2252,7 +2252,7 @@
     </row>
     <row r="52" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B52" s="42">
         <v>1199600</v>
@@ -2261,7 +2261,7 @@
         <v>1311723</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E52" s="38"/>
       <c r="F52" s="38"/>
@@ -2282,7 +2282,7 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2305,7 +2305,7 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B55" s="56"/>
       <c r="C55" s="56"/>
@@ -2331,20 +2331,20 @@
         <v>16652</v>
       </c>
       <c r="B56" s="44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D56" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E56" s="21"/>
       <c r="F56" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="G56" s="21" t="s">
         <v>72</v>
-      </c>
-      <c r="G56" s="21" t="s">
-        <v>73</v>
       </c>
       <c r="H56" s="48"/>
       <c r="I56" s="24">
@@ -2361,20 +2361,20 @@
         <v>16849</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C57" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D57" s="50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E57" s="21"/>
       <c r="F57" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G57" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H57" s="48"/>
       <c r="I57" s="24">
@@ -2391,20 +2391,20 @@
         <v>16879</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C58" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D58" s="50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E58" s="21"/>
       <c r="F58" s="47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G58" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H58" s="48"/>
       <c r="I58" s="24">
@@ -2418,7 +2418,7 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B61" s="56"/>
       <c r="C61" s="56"/>
@@ -2473,7 +2473,7 @@
         <v>28193</v>
       </c>
       <c r="D62" s="53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E62" s="53"/>
       <c r="F62" s="23"/>
@@ -2506,7 +2506,7 @@
         <v>17157</v>
       </c>
       <c r="D63" s="53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E63" s="53"/>
       <c r="F63" s="23"/>
@@ -2539,7 +2539,7 @@
         <v>1305382</v>
       </c>
       <c r="D64" s="53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E64" s="53"/>
       <c r="F64" s="23"/>
@@ -2563,16 +2563,16 @@
     </row>
     <row r="65" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B65" s="23">
         <v>5210291</v>
       </c>
       <c r="C65" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="53" t="s">
         <v>83</v>
-      </c>
-      <c r="D65" s="53" t="s">
-        <v>84</v>
       </c>
       <c r="E65" s="53"/>
       <c r="F65" s="23"/>
@@ -2596,7 +2596,7 @@
     </row>
     <row r="66" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B66" s="23">
         <v>5436789</v>
@@ -2605,7 +2605,7 @@
         <v>1299187</v>
       </c>
       <c r="D66" s="53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E66" s="53"/>
       <c r="F66" s="23"/>
@@ -2647,23 +2647,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E86FB901-2D43-49F7-AF25-C8E3CE6F969E}" scale="93" topLeftCell="A48">
-      <selection activeCell="D57" sqref="D57"/>
+    <customSheetView guid="{EB0EC4D1-8B8D-46FB-BC39-0BA2397624AA}" scale="80">
+      <selection activeCell="A135" sqref="A135"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{89EB5726-03E5-4F2C-A6BE-9D2A424F6109}" scale="80" topLeftCell="A79">
+      <selection activeCell="D115" sqref="D115"/>
+      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{C156F9C8-FAC6-485D-BA71-3158CC8B4510}" scale="80" showPageBreaks="1" fitToPage="1">
       <selection activeCell="I35" sqref="I35"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <pageSetup paperSize="9" scale="14" orientation="portrait" r:id="rId2"/>
+      <pageSetup paperSize="9" scale="14" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{89EB5726-03E5-4F2C-A6BE-9D2A424F6109}" scale="80" topLeftCell="A79">
-      <selection activeCell="D115" sqref="D115"/>
-      <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-    </customSheetView>
-    <customSheetView guid="{EB0EC4D1-8B8D-46FB-BC39-0BA2397624AA}" scale="80">
-      <selection activeCell="A135" sqref="A135"/>
+    <customSheetView guid="{E86FB901-2D43-49F7-AF25-C8E3CE6F969E}" scale="93" topLeftCell="A48">
+      <selection activeCell="D57" sqref="D57"/>
       <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -2697,6 +2697,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x010100F2D1A7DA3F5F5E4BAFF1526146277863" ma:contentTypeVersion="9" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="cae959bd6a21d0dfda98c3a403ef169a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0cb0dbfe-2770-4c8a-831b-00a16f8a3714" xmlns:ns3="b3540951-9d5f-467b-9604-bb49f037c0fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f3d3368b13bdc6e21385adbc53e96e1" ns2:_="" ns3:_="">
     <xsd:import namespace="0cb0dbfe-2770-4c8a-831b-00a16f8a3714"/>
@@ -2893,15 +2902,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2909,6 +2909,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9311EABC-5B22-437F-A7AE-A68972931720}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F137572C-0560-46EB-967B-149C1E95252E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2923,14 +2931,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9311EABC-5B22-437F-A7AE-A68972931720}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>